<commit_message>
can print the whole list now
</commit_message>
<xml_diff>
--- a/Apenator.xlsx
+++ b/Apenator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wujieyan/git/Apenator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8EDFC1-238E-524D-BA99-FB0F6FC5EDDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{263E10E9-BCC9-1C42-9EF4-37EB16F54849}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12840" yWindow="0" windowWidth="12760" windowHeight="16000" xr2:uid="{B923F371-3C33-B243-B632-EE30ABCFC764}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="95">
   <si>
     <t>Name</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Tail</t>
   </si>
   <si>
-    <t>Lemurs</t>
-  </si>
-  <si>
     <t>Squirrel Monkey</t>
   </si>
   <si>
@@ -141,9 +138,6 @@
     <t>carnivorous</t>
   </si>
   <si>
-    <t>Lorises</t>
-  </si>
-  <si>
     <t>nocturnal and diurnal</t>
   </si>
   <si>
@@ -177,9 +171,6 @@
     <t>black</t>
   </si>
   <si>
-    <t>omnivores</t>
-  </si>
-  <si>
     <t>black-white</t>
   </si>
   <si>
@@ -213,9 +204,6 @@
     <t>bloned-red</t>
   </si>
   <si>
-    <t>Galagos</t>
-  </si>
-  <si>
     <t>category</t>
   </si>
   <si>
@@ -316,6 +304,18 @@
   </si>
   <si>
     <t>abroreal</t>
+  </si>
+  <si>
+    <t>Loris</t>
+  </si>
+  <si>
+    <t>gray-brown</t>
+  </si>
+  <si>
+    <t>Lemur</t>
+  </si>
+  <si>
+    <t>Galago</t>
   </si>
 </sst>
 </file>
@@ -360,8 +360,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -679,7 +679,7 @@
   <dimension ref="A1:S27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -693,7 +693,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -702,7 +702,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -729,54 +729,54 @@
         <v>10</v>
       </c>
       <c r="N1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="Q1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" t="s">
-        <v>29</v>
-      </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F2">
         <v>2133</v>
       </c>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="L2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="M2">
         <v>1</v>
@@ -793,40 +793,40 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F3">
         <v>2133</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="L3" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="M3">
         <v>1</v>
@@ -841,45 +841,45 @@
         <v>0</v>
       </c>
       <c r="Q3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F4">
         <v>2133</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M4">
         <v>1</v>
@@ -896,40 +896,40 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F5">
         <v>2133</v>
       </c>
       <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" t="s">
         <v>45</v>
       </c>
-      <c r="H5" t="s">
-        <v>48</v>
-      </c>
-      <c r="I5" t="s">
-        <v>43</v>
-      </c>
-      <c r="J5" t="s">
-        <v>47</v>
-      </c>
       <c r="K5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M5">
         <v>1</v>
@@ -946,40 +946,40 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F6">
         <v>2133</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H6" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="I6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="K6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M6">
         <v>1</v>
@@ -994,98 +994,98 @@
         <v>0</v>
       </c>
       <c r="Q6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F7">
         <v>2133</v>
       </c>
       <c r="G7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="K7" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="s">
         <v>65</v>
-      </c>
-      <c r="L7" t="s">
-        <v>40</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>1</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F8">
         <v>2133</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H8" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="I8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="K8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="L8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M8">
         <v>1</v>
@@ -1100,42 +1100,42 @@
         <v>0</v>
       </c>
       <c r="Q8" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F9">
         <v>2133</v>
       </c>
       <c r="G9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H9" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="K9" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M9">
         <v>1</v>
@@ -1150,45 +1150,45 @@
         <v>0</v>
       </c>
       <c r="Q9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F10">
         <v>2123</v>
       </c>
       <c r="G10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="K10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -1202,46 +1202,46 @@
       <c r="P10">
         <v>1</v>
       </c>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F11">
         <v>2123</v>
       </c>
       <c r="G11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K11" t="s">
+        <v>67</v>
+      </c>
+      <c r="L11" t="s">
         <v>31</v>
       </c>
-      <c r="K11" t="s">
-        <v>71</v>
-      </c>
-      <c r="L11" t="s">
-        <v>32</v>
-      </c>
       <c r="M11">
         <v>0</v>
       </c>
@@ -1254,45 +1254,45 @@
       <c r="P11">
         <v>1</v>
       </c>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D12">
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F12">
         <v>2123</v>
       </c>
       <c r="G12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" t="s">
+        <v>26</v>
+      </c>
+      <c r="J12" t="s">
         <v>45</v>
       </c>
-      <c r="H12" t="s">
-        <v>48</v>
-      </c>
-      <c r="I12" t="s">
-        <v>27</v>
-      </c>
-      <c r="J12" t="s">
-        <v>47</v>
-      </c>
       <c r="K12" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="L12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -1307,45 +1307,45 @@
         <v>1</v>
       </c>
       <c r="Q12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F13">
         <v>2123</v>
       </c>
       <c r="G13" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H13" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="I13" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J13" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" t="s">
+        <v>74</v>
+      </c>
+      <c r="L13" t="s">
         <v>31</v>
-      </c>
-      <c r="K13" t="s">
-        <v>78</v>
-      </c>
-      <c r="L13" t="s">
-        <v>32</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -1362,40 +1362,40 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F14">
         <v>2123</v>
       </c>
       <c r="G14" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" t="s">
+        <v>75</v>
+      </c>
+      <c r="I14" t="s">
+        <v>26</v>
+      </c>
+      <c r="J14" t="s">
         <v>45</v>
       </c>
-      <c r="H14" t="s">
-        <v>79</v>
-      </c>
-      <c r="I14" t="s">
-        <v>27</v>
-      </c>
-      <c r="J14" t="s">
-        <v>47</v>
-      </c>
       <c r="K14" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="L14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -1412,40 +1412,40 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F15">
         <v>2123</v>
       </c>
       <c r="G15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J15" t="s">
+        <v>30</v>
+      </c>
+      <c r="K15" t="s">
+        <v>61</v>
+      </c>
+      <c r="L15" t="s">
         <v>31</v>
-      </c>
-      <c r="K15" t="s">
-        <v>65</v>
-      </c>
-      <c r="L15" t="s">
-        <v>32</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -1462,40 +1462,40 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D16">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F16">
         <v>2123</v>
       </c>
       <c r="G16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H16" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J16" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="K16" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="L16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M16">
         <v>1</v>
@@ -1512,40 +1512,40 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>70</v>
+        <v>20</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F17">
         <v>2123</v>
       </c>
       <c r="G17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I17" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="J17" t="s">
+        <v>30</v>
+      </c>
+      <c r="K17" t="s">
+        <v>84</v>
+      </c>
+      <c r="L17" t="s">
         <v>31</v>
-      </c>
-      <c r="K17" t="s">
-        <v>88</v>
-      </c>
-      <c r="L17" t="s">
-        <v>32</v>
       </c>
       <c r="M17">
         <v>0</v>
@@ -1562,31 +1562,31 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>70</v>
+        <v>21</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F18">
         <v>2123</v>
       </c>
       <c r="I18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K18" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="L18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M18">
         <v>1</v>
@@ -1600,40 +1600,40 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F19">
         <v>2123</v>
       </c>
       <c r="G19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I19" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J19" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="K19" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="L19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M19">
         <v>1</v>
@@ -1645,45 +1645,45 @@
         <v>0</v>
       </c>
       <c r="Q19" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F20">
         <v>2123</v>
       </c>
       <c r="G20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H20" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="K20" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="L20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M20">
         <v>1</v>
@@ -1700,53 +1700,107 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" t="s">
         <v>28</v>
       </c>
-      <c r="C21" t="s">
-        <v>29</v>
+      <c r="D21">
+        <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="F21">
+        <v>2133</v>
       </c>
       <c r="G21" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="H21" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="I21" t="s">
-        <v>27</v>
+        <v>47</v>
+      </c>
+      <c r="J21" t="s">
+        <v>92</v>
+      </c>
+      <c r="K21" t="s">
+        <v>60</v>
+      </c>
+      <c r="L21" t="s">
+        <v>38</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22">
+        <v>2133</v>
+      </c>
+      <c r="G22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" t="s">
+        <v>75</v>
+      </c>
+      <c r="I22" t="s">
+        <v>36</v>
+      </c>
+      <c r="J22" t="s">
+        <v>80</v>
+      </c>
+      <c r="K22" t="s">
         <v>60</v>
       </c>
-      <c r="B22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" t="s">
-        <v>26</v>
-      </c>
-      <c r="H22" t="s">
-        <v>31</v>
-      </c>
-      <c r="I22" t="s">
+      <c r="L22" t="s">
         <v>38</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>